<commit_message>
Mise a jour JE
il reste tblplateformeJeu a finir et vérifier un truc sur
tblJeuSemblable
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Dropbox\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Utilisateur\Dropbox\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tblMode" sheetId="1" r:id="rId1"/>
     <sheet name="tblTheme" sheetId="2" r:id="rId2"/>
     <sheet name="tblJeu" sheetId="3" r:id="rId3"/>
+    <sheet name="tblThemeJeu" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="383">
   <si>
     <t>IdMode</t>
   </si>
@@ -1172,6 +1173,9 @@
   </si>
   <si>
     <t>NHL 14 est un jeu de hockey sur glace. Le joueur peut s'y prendre pour un professionnel et gérer sa propre carrière ou bien gérer l'avenir d'une franchise dans le mode DG. Des matchs old-school inspirés par NHL 94 sont également au programme.</t>
+  </si>
+  <si>
+    <t>Heroic-fantaisy</t>
   </si>
 </sst>
 </file>
@@ -1520,13 +1524,13 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="106.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="106.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1537,7 +1541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="16.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1548,7 +1552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1559,7 +1563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1570,7 +1574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1589,18 +1593,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C347"/>
+  <dimension ref="A1:C337"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A282" workbookViewId="0">
+      <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1611,7 +1615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1619,7 +1623,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1627,7 +1631,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1635,7 +1639,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1643,7 +1647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1651,7 +1655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1659,7 +1663,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1667,7 +1671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1675,7 +1679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1683,7 +1687,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1691,7 +1695,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1699,7 +1703,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1707,7 +1711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1715,7 +1719,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1723,7 +1727,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1731,7 +1735,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1739,7 +1743,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1747,7 +1751,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1755,7 +1759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1763,7 +1767,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1771,7 +1775,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1779,7 +1783,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1787,7 +1791,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1795,7 +1799,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1803,7 +1807,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1811,7 +1815,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1819,7 +1823,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1827,7 +1831,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1835,7 +1839,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1843,7 +1847,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1851,7 +1855,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1859,7 +1863,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1867,7 +1871,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1875,7 +1879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1883,7 +1887,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1891,7 +1895,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1899,7 +1903,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1907,7 +1911,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1915,7 +1919,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1923,7 +1927,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1931,7 +1935,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1939,7 +1943,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1947,7 +1951,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1955,7 +1959,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1963,7 +1967,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1971,7 +1975,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1979,7 +1983,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1987,7 +1991,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1995,7 +1999,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2003,7 +2007,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2011,7 +2015,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2019,7 +2023,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2027,7 +2031,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2035,7 +2039,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2043,7 +2047,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2051,7 +2055,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2059,7 +2063,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2067,7 +2071,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2075,7 +2079,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2083,7 +2087,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2091,7 +2095,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2099,7 +2103,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2107,7 +2111,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2115,7 +2119,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2123,7 +2127,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2131,7 +2135,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2139,7 +2143,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2147,7 +2151,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2155,7 +2159,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2163,7 +2167,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2171,7 +2175,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2179,7 +2183,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2187,7 +2191,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2195,7 +2199,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2203,7 +2207,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2211,7 +2215,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2219,7 +2223,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2227,7 +2231,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2235,7 +2239,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2243,7 +2247,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2251,7 +2255,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2259,7 +2263,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2267,7 +2271,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2275,7 +2279,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2283,7 +2287,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2291,7 +2295,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2299,7 +2303,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2307,7 +2311,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2315,7 +2319,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2323,7 +2327,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2331,7 +2335,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2339,7 +2343,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2347,7 +2351,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2355,7 +2359,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2363,7 +2367,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2371,7 +2375,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2379,7 +2383,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2387,7 +2391,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2395,7 +2399,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2403,7 +2407,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2411,7 +2415,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2419,7 +2423,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2427,7 +2431,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2435,7 +2439,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2443,7 +2447,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2451,7 +2455,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2459,7 +2463,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2467,7 +2471,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2475,7 +2479,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2483,7 +2487,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2491,7 +2495,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2499,7 +2503,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2507,7 +2511,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2515,7 +2519,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2523,7 +2527,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2531,7 +2535,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2539,7 +2543,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2547,7 +2551,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2555,7 +2559,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2563,7 +2567,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2571,7 +2575,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2579,7 +2583,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2587,7 +2591,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2595,7 +2599,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2603,7 +2607,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2611,7 +2615,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -2619,7 +2623,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -2627,7 +2631,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -2635,7 +2639,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -2643,7 +2647,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -2651,7 +2655,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -2659,7 +2663,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -2667,7 +2671,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -2675,7 +2679,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -2683,7 +2687,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -2691,7 +2695,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -2699,7 +2703,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -2707,7 +2711,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -2715,7 +2719,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -2723,7 +2727,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -2731,7 +2735,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -2739,7 +2743,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -2747,7 +2751,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -2755,7 +2759,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -2763,7 +2767,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -2771,7 +2775,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -2779,7 +2783,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -2787,7 +2791,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -2795,7 +2799,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -2803,7 +2807,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -2811,7 +2815,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -2819,7 +2823,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -2827,7 +2831,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -2835,7 +2839,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -2843,7 +2847,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -2851,7 +2855,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -2859,7 +2863,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -2867,7 +2871,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -2875,7 +2879,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -2883,7 +2887,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -2891,7 +2895,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -2899,7 +2903,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -2907,311 +2911,311 @@
         <v>175</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -3219,1131 +3223,1084 @@
         <v>213</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>238</v>
       </c>
       <c r="B239" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>239</v>
       </c>
       <c r="B240" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>240</v>
       </c>
       <c r="B241" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>241</v>
       </c>
       <c r="B242" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>242</v>
       </c>
       <c r="B243" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>243</v>
       </c>
       <c r="B244" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>244</v>
       </c>
       <c r="B245" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>245</v>
       </c>
       <c r="B246" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>246</v>
       </c>
       <c r="B247" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>247</v>
       </c>
       <c r="B248" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>248</v>
       </c>
       <c r="B249" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>249</v>
       </c>
       <c r="B250" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>
       <c r="B251" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>251</v>
       </c>
       <c r="B252" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>252</v>
       </c>
       <c r="B253" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>253</v>
       </c>
       <c r="B254" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>254</v>
       </c>
       <c r="B255" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>255</v>
       </c>
       <c r="B256" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>256</v>
       </c>
       <c r="B257" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>257</v>
       </c>
       <c r="B258" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>258</v>
       </c>
       <c r="B259" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>259</v>
       </c>
       <c r="B260" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>260</v>
       </c>
       <c r="B261" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>261</v>
       </c>
       <c r="B262" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>262</v>
       </c>
       <c r="B263" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>263</v>
       </c>
       <c r="B264" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>264</v>
       </c>
       <c r="B265" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>265</v>
       </c>
       <c r="B266" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>266</v>
       </c>
       <c r="B267" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>267</v>
       </c>
       <c r="B268" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>268</v>
       </c>
       <c r="B269" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>269</v>
       </c>
       <c r="B270" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>270</v>
       </c>
       <c r="B271" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>271</v>
       </c>
       <c r="B272" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>272</v>
       </c>
       <c r="B273" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>273</v>
       </c>
       <c r="B274" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>274</v>
       </c>
       <c r="B275" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>275</v>
       </c>
       <c r="B276" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>276</v>
       </c>
       <c r="B277" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>277</v>
       </c>
       <c r="B278" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>278</v>
       </c>
       <c r="B279" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>279</v>
       </c>
       <c r="B280" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>280</v>
       </c>
       <c r="B281" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>281</v>
       </c>
       <c r="B282" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>282</v>
       </c>
       <c r="B283" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>283</v>
       </c>
       <c r="B284" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>284</v>
       </c>
       <c r="B285" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>285</v>
       </c>
       <c r="B286" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>286</v>
       </c>
       <c r="B287" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>287</v>
       </c>
       <c r="B288" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>288</v>
       </c>
       <c r="B289" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>289</v>
       </c>
       <c r="B290" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>290</v>
       </c>
       <c r="B291" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>291</v>
       </c>
       <c r="B292" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>292</v>
       </c>
       <c r="B293" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>293</v>
       </c>
       <c r="B294" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>294</v>
       </c>
       <c r="B295" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>295</v>
       </c>
       <c r="B296" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>296</v>
       </c>
       <c r="B297" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>297</v>
       </c>
       <c r="B298" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>298</v>
       </c>
       <c r="B299" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>299</v>
       </c>
       <c r="B300" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>300</v>
       </c>
       <c r="B301" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>301</v>
       </c>
       <c r="B302" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>302</v>
       </c>
       <c r="B303" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>303</v>
       </c>
       <c r="B304" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>304</v>
       </c>
       <c r="B305" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>305</v>
       </c>
       <c r="B306" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>306</v>
       </c>
       <c r="B307" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>307</v>
       </c>
       <c r="B308" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>308</v>
       </c>
       <c r="B309" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>309</v>
       </c>
       <c r="B310" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>310</v>
       </c>
       <c r="B311" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>311</v>
       </c>
       <c r="B312" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>312</v>
       </c>
       <c r="B313" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>313</v>
       </c>
       <c r="B314" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>314</v>
       </c>
       <c r="B315" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>315</v>
       </c>
       <c r="B316" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>316</v>
       </c>
       <c r="B317" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>317</v>
       </c>
       <c r="B318" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>318</v>
       </c>
       <c r="B319" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>319</v>
       </c>
       <c r="B320" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>320</v>
       </c>
       <c r="B321" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>321</v>
       </c>
       <c r="B322" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>322</v>
       </c>
       <c r="B323" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>323</v>
       </c>
       <c r="B324" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>324</v>
       </c>
       <c r="B325" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>325</v>
       </c>
       <c r="B326" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>326</v>
       </c>
       <c r="B327" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>327</v>
       </c>
       <c r="B328" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>328</v>
       </c>
       <c r="B329" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>329</v>
       </c>
       <c r="B330" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>330</v>
       </c>
       <c r="B331" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>331</v>
       </c>
       <c r="B332" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>332</v>
       </c>
       <c r="B333" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>333</v>
       </c>
       <c r="B334" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>334</v>
       </c>
       <c r="B335" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>335</v>
       </c>
       <c r="B336" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>336</v>
       </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A338">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A339">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A340">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A341">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A342">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A343">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A344">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A345">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A346">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A347">
-        <v>346</v>
+      <c r="B337" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -4355,17 +4312,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="229.77734375" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
+    <col min="3" max="3" width="229.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>348</v>
       </c>
@@ -4391,7 +4348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4414,7 +4371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4437,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4460,7 +4417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4483,7 +4440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4506,7 +4463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4529,7 +4486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4552,7 +4509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4575,7 +4532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4598,7 +4555,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4621,7 +4578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4644,7 +4601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4667,7 +4624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4690,7 +4647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4713,7 +4670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4740,4 +4697,187 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>296</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Élo veux pas que je me suicide
update JE
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="tblMode" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="413">
   <si>
     <t>IdMode</t>
   </si>
@@ -1193,36 +1193,12 @@
     <t>IdPlateforme</t>
   </si>
   <si>
-    <t>PS3</t>
-  </si>
-  <si>
-    <t>PS4</t>
-  </si>
-  <si>
-    <t>ONE</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>Mac</t>
-  </si>
-  <si>
-    <t>WiiU</t>
-  </si>
-  <si>
-    <t>iOS</t>
-  </si>
-  <si>
     <t>solo + multi ?</t>
   </si>
   <si>
     <t>CoteESRB</t>
   </si>
   <si>
-    <t>pc</t>
-  </si>
-  <si>
     <t>CodeVersion</t>
   </si>
   <si>
@@ -1250,10 +1226,49 @@
     <t>darkest dungeon 1.0</t>
   </si>
   <si>
-    <t>1er verison suite au financement kickstarter, version de départ</t>
-  </si>
-  <si>
     <t>Alpha</t>
+  </si>
+  <si>
+    <t>DarkDn02</t>
+  </si>
+  <si>
+    <t>darkest dungeon 1.1</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>FTL01</t>
+  </si>
+  <si>
+    <t>faster than light 1.0</t>
+  </si>
+  <si>
+    <t>FTL02</t>
+  </si>
+  <si>
+    <t>faster than light 1.1</t>
+  </si>
+  <si>
+    <t>1er version suite au financement kickstarter, version de départ, beaucoup de bug</t>
+  </si>
+  <si>
+    <t>1er version suite au financement kickstarter, version de départ</t>
+  </si>
+  <si>
+    <t>2e version mise a jour des bug, ajoute de classe, bosse, ennemis, et nouveau niveau</t>
+  </si>
+  <si>
+    <t>2e versions, bug corriger, ajout de vaisseau et d'évènment aléatoire</t>
+  </si>
+  <si>
+    <t>FTL03</t>
+  </si>
+  <si>
+    <t>faster than light 1.2</t>
+  </si>
+  <si>
+    <t>3e versions final, dernier bug, ajout de vaisseau et d'évènment aléatoire</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1335,19 +1350,6 @@
       <left style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </right>
@@ -1413,7 +1415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1424,19 +1426,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1794,7 +1790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C337"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A334" workbookViewId="0">
       <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
@@ -4538,7 +4534,7 @@
         <v>352</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>353</v>
@@ -5159,7 +5155,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -5179,8 +5175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5198,275 +5194,251 @@
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>396</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>2</v>
       </c>
-      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>3</v>
       </c>
-      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>388</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>1</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="4" t="s">
-        <v>391</v>
+      <c r="B6" s="7">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <v>2</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>1</v>
       </c>
-      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <v>2</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>2</v>
       </c>
-      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>2</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>3</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>390</v>
-      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="A10" s="9">
         <v>2</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="9">
         <v>2</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>7</v>
       </c>
-      <c r="C11" s="10"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
+      <c r="A12" s="9">
         <v>2</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>8</v>
       </c>
-      <c r="C12" s="10"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="8">
         <v>9</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>391</v>
+      <c r="B14" s="8">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
-      <c r="C15" s="4">
-        <v>360</v>
+      <c r="B15" s="8">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
-      <c r="C17" s="4"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>7</v>
       </c>
-      <c r="C19" s="4"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>8</v>
       </c>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="12">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>9</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" s="4"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>9</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>10</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="C26" s="4"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
       <c r="B27">
         <v>3</v>
       </c>
-      <c r="C27" s="4"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10</v>
       </c>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>11</v>
       </c>
       <c r="B29">
         <v>12</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>11</v>
       </c>
       <c r="B30">
         <v>14</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>11</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>11</v>
       </c>
-      <c r="C32" s="4">
-        <v>360</v>
+      <c r="B32">
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -5476,7 +5448,6 @@
       <c r="B33">
         <v>12</v>
       </c>
-      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -5485,19 +5456,22 @@
       <c r="B34">
         <v>14</v>
       </c>
-      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>12</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="B35">
+        <v>15</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>12</v>
       </c>
-      <c r="C36" s="4"/>
+      <c r="B36">
+        <v>16</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
@@ -5506,7 +5480,6 @@
       <c r="B37">
         <v>12</v>
       </c>
-      <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
@@ -5515,56 +5488,70 @@
       <c r="B38">
         <v>14</v>
       </c>
-      <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>13</v>
       </c>
-      <c r="C39" s="4"/>
+      <c r="B39">
+        <v>15</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>13</v>
       </c>
-      <c r="C40" s="4"/>
+      <c r="B40">
+        <v>16</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>14</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>387</v>
+      <c r="B41">
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>14</v>
       </c>
-      <c r="C42" s="4">
-        <v>360</v>
+      <c r="B42">
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>15</v>
       </c>
-      <c r="C43" s="4"/>
+      <c r="B43">
+        <v>15</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>15</v>
       </c>
+      <c r="B44">
+        <v>16</v>
+      </c>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>16</v>
       </c>
+      <c r="B45">
+        <v>15</v>
+      </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
+        <v>16</v>
+      </c>
+      <c r="B46">
         <v>16</v>
       </c>
       <c r="C46" s="4"/>
@@ -5579,56 +5566,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="55" customWidth="1"/>
+    <col min="3" max="3" width="78.33203125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="6" max="6" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>398</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>399</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>400</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>401</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>402</v>
-      </c>
-      <c r="G1" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>391</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>392</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>352</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>403</v>
+      <c r="H1" s="11" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B2" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="C2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D2" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
       <c r="E2">
         <v>20140214</v>
@@ -5640,8 +5627,100 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B3" t="s">
+        <v>400</v>
+      </c>
+      <c r="C3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D3" t="s">
+        <v>401</v>
+      </c>
+      <c r="E3">
+        <v>20150720</v>
+      </c>
+      <c r="F3">
+        <v>20151212</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B4" t="s">
+        <v>403</v>
+      </c>
+      <c r="C4" t="s">
+        <v>406</v>
+      </c>
+      <c r="D4" t="s">
+        <v>401</v>
+      </c>
+      <c r="E4">
+        <v>20130916</v>
+      </c>
+      <c r="F4">
+        <v>20140320</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>404</v>
+      </c>
+      <c r="B5" t="s">
+        <v>405</v>
+      </c>
+      <c r="C5" t="s">
+        <v>409</v>
+      </c>
+      <c r="D5" t="s">
+        <v>401</v>
+      </c>
+      <c r="E5">
+        <v>20140101</v>
+      </c>
+      <c r="F5">
+        <v>20140320</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" t="s">
+        <v>411</v>
+      </c>
+      <c r="C6" t="s">
+        <v>412</v>
+      </c>
+      <c r="D6" t="s">
+        <v>401</v>
+      </c>
+      <c r="E6">
+        <v>20140101</v>
+      </c>
+      <c r="F6">
+        <v>20140320</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I15" s="8"/>
+      <c r="I15" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
JE tblversion base terminer
tout est là mais je crois qu'il faudrait revoir le nombre de caractère
du nom de version !!!!!!!!!
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Dropbox\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Utilisateur\Dropbox\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="633" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" tabRatio="633" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="tblMode" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="494">
   <si>
     <t>IdMode</t>
   </si>
@@ -1347,6 +1347,171 @@
   </si>
   <si>
     <t>3e version du Multi local de halo 4, nouvelle map et nouveau mode de jeux</t>
+  </si>
+  <si>
+    <t>MKart8SS01</t>
+  </si>
+  <si>
+    <t>Mario Kart 8 solo 1.0</t>
+  </si>
+  <si>
+    <t>1er version du solo de Mario Kart 8, bug nombreux</t>
+  </si>
+  <si>
+    <t>MKart8SS02</t>
+  </si>
+  <si>
+    <t>Mario Kart 8 solo 1.1</t>
+  </si>
+  <si>
+    <t>MKart8ML01</t>
+  </si>
+  <si>
+    <t>MKart8ML02</t>
+  </si>
+  <si>
+    <t>Mario Kart 8 Multi Local 1.0</t>
+  </si>
+  <si>
+    <t>Mario Kart 8 Multi Local 1.1</t>
+  </si>
+  <si>
+    <t>1er version du Multi Local de Mario Kart 8, bug nombreux</t>
+  </si>
+  <si>
+    <t>MKart8MO01</t>
+  </si>
+  <si>
+    <t>MKart8MO02</t>
+  </si>
+  <si>
+    <t>1er version du Multi en ligne de Mario Kart 8, bug nombreux</t>
+  </si>
+  <si>
+    <t>2er version du solo de Mario Kart 8, ajout mode course, mini-jeux, etc</t>
+  </si>
+  <si>
+    <t>2er version du Multi Local de Mario Kart 8, ajout mode course, mini-jeux, etc</t>
+  </si>
+  <si>
+    <t>2er version du Multi en ligne de Mario Kart 8, ajout mode course, mini-jeux, etc</t>
+  </si>
+  <si>
+    <t>Mario Kart 8 Multi online 1.1</t>
+  </si>
+  <si>
+    <t>Mario Kart 8 Multi online 1.0</t>
+  </si>
+  <si>
+    <t>Max taille CodeVersion</t>
+  </si>
+  <si>
+    <t>WOW01</t>
+  </si>
+  <si>
+    <t>world of warcraft 1.0</t>
+  </si>
+  <si>
+    <t>1er version d'essaie du openworld, nombreux crash serveur et bug joueur</t>
+  </si>
+  <si>
+    <t>WOW02</t>
+  </si>
+  <si>
+    <t>world of warcraft 1.1</t>
+  </si>
+  <si>
+    <t>2e version, ajout des donjons, des évènement aléatoire, du craft et etc.</t>
+  </si>
+  <si>
+    <t>WOWCT01</t>
+  </si>
+  <si>
+    <t>world of warcraft CT  1.0</t>
+  </si>
+  <si>
+    <t>1e version d'extension, Refonte du monde, nouvelle classe, race, lieux, etc.</t>
+  </si>
+  <si>
+    <t>NHL15SS01</t>
+  </si>
+  <si>
+    <t>NHL 15 solo 1.0</t>
+  </si>
+  <si>
+    <t>1er version, nouveau joueur, peu de bug, ressemblance avec NHL 2014</t>
+  </si>
+  <si>
+    <t>NHL15SS02</t>
+  </si>
+  <si>
+    <t>NHL 15 solo 1.1</t>
+  </si>
+  <si>
+    <t>2e version, nouveau chandaille, nouveau commentateur</t>
+  </si>
+  <si>
+    <t>NHL15ML01</t>
+  </si>
+  <si>
+    <t>NHL15ML02</t>
+  </si>
+  <si>
+    <t>NHL15MO02</t>
+  </si>
+  <si>
+    <t>NHL15MO01</t>
+  </si>
+  <si>
+    <t>NHL 15 Multi Local 1.0</t>
+  </si>
+  <si>
+    <t>NHL 15 Multi Local 1.1</t>
+  </si>
+  <si>
+    <t>NHL 15 Multi en ligne 1.0</t>
+  </si>
+  <si>
+    <t>NHL 15 Multi en ligne 1.1</t>
+  </si>
+  <si>
+    <t>NHL14SS01</t>
+  </si>
+  <si>
+    <t>NHL14SS02</t>
+  </si>
+  <si>
+    <t>NHL14ML01</t>
+  </si>
+  <si>
+    <t>NHL14ML02</t>
+  </si>
+  <si>
+    <t>NHL14MO01</t>
+  </si>
+  <si>
+    <t>NHL14MO02</t>
+  </si>
+  <si>
+    <t>NHL 14 solo 1.0</t>
+  </si>
+  <si>
+    <t>NHL 14 solo 1.1</t>
+  </si>
+  <si>
+    <t>NHL 14 Multi Local 1.0</t>
+  </si>
+  <si>
+    <t>NHL 14 Multi Local 1.1</t>
+  </si>
+  <si>
+    <t>NHL 14 Multi en ligne 1.0</t>
+  </si>
+  <si>
+    <t>NHL 14 Multi en ligne 1.1</t>
+  </si>
+  <si>
+    <t>1er version, nouveau joueur, peu de bug, ressemblance avec NHL 2013</t>
   </si>
 </sst>
 </file>
@@ -1797,13 +1962,13 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.6640625" customWidth="1"/>
-    <col min="3" max="3" width="106.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="106.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1814,7 +1979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="16.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1825,7 +1990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1836,7 +2001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1847,7 +2012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1872,12 +2037,12 @@
       <selection activeCell="C165" sqref="C165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1888,7 +2053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1896,7 +2061,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1904,7 +2069,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1912,7 +2077,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1920,7 +2085,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1928,7 +2093,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1936,7 +2101,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1944,7 +2109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1952,7 +2117,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1960,7 +2125,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1968,7 +2133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1976,7 +2141,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1984,7 +2149,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1992,7 +2157,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2000,7 +2165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2008,7 +2173,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2016,7 +2181,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2024,7 +2189,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2032,7 +2197,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2040,7 +2205,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2048,7 +2213,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2056,7 +2221,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2064,7 +2229,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2072,7 +2237,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2080,7 +2245,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2088,7 +2253,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2096,7 +2261,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2104,7 +2269,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2112,7 +2277,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2120,7 +2285,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2128,7 +2293,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2136,7 +2301,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2144,7 +2309,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2152,7 +2317,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2160,7 +2325,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2168,7 +2333,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2176,7 +2341,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2184,7 +2349,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2192,7 +2357,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2200,7 +2365,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2208,7 +2373,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2216,7 +2381,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2224,7 +2389,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2232,7 +2397,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2240,7 +2405,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2248,7 +2413,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2256,7 +2421,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2264,7 +2429,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2272,7 +2437,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2280,7 +2445,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2288,7 +2453,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2296,7 +2461,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2304,7 +2469,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2312,7 +2477,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2320,7 +2485,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2328,7 +2493,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2336,7 +2501,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2344,7 +2509,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2352,7 +2517,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2360,7 +2525,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2368,7 +2533,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2376,7 +2541,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2384,7 +2549,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2392,7 +2557,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2400,7 +2565,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2408,7 +2573,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2416,7 +2581,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2424,7 +2589,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2432,7 +2597,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2440,7 +2605,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2448,7 +2613,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2456,7 +2621,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2464,7 +2629,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2472,7 +2637,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2480,7 +2645,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2488,7 +2653,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2496,7 +2661,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2504,7 +2669,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2512,7 +2677,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2520,7 +2685,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2528,7 +2693,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2536,7 +2701,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2544,7 +2709,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2552,7 +2717,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2560,7 +2725,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2568,7 +2733,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2576,7 +2741,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2584,7 +2749,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2592,7 +2757,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2600,7 +2765,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2608,7 +2773,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2616,7 +2781,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2624,7 +2789,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2632,7 +2797,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2640,7 +2805,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2648,7 +2813,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2656,7 +2821,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2664,7 +2829,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2672,7 +2837,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2680,7 +2845,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2688,7 +2853,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2696,7 +2861,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2704,7 +2869,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2712,7 +2877,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2720,7 +2885,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2728,7 +2893,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2736,7 +2901,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2744,7 +2909,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2752,7 +2917,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2760,7 +2925,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2768,7 +2933,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2776,7 +2941,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2784,7 +2949,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2792,7 +2957,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2800,7 +2965,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2808,7 +2973,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2816,7 +2981,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2824,7 +2989,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2832,7 +2997,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2840,7 +3005,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2848,7 +3013,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2856,7 +3021,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2864,7 +3029,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2872,7 +3037,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2880,7 +3045,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2888,7 +3053,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -2896,7 +3061,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -2904,7 +3069,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -2912,7 +3077,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -2920,7 +3085,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -2928,7 +3093,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -2936,7 +3101,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -2944,7 +3109,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -2952,7 +3117,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -2960,7 +3125,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -2968,7 +3133,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -2976,7 +3141,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -2984,7 +3149,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -2992,7 +3157,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -3000,7 +3165,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -3008,7 +3173,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -3016,7 +3181,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -3024,7 +3189,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -3032,7 +3197,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3040,7 +3205,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -3048,7 +3213,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -3056,7 +3221,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -3064,7 +3229,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -3072,7 +3237,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -3080,7 +3245,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -3088,7 +3253,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -3096,7 +3261,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -3104,7 +3269,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -3112,7 +3277,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -3120,7 +3285,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -3128,7 +3293,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -3136,7 +3301,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -3144,7 +3309,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -3152,7 +3317,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -3160,7 +3325,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -3168,7 +3333,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -3176,7 +3341,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -3184,7 +3349,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -3192,7 +3357,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -3200,7 +3365,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -3208,7 +3373,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -3216,7 +3381,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -3224,7 +3389,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -3232,7 +3397,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -3240,7 +3405,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -3248,7 +3413,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -3256,7 +3421,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -3264,7 +3429,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -3272,7 +3437,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -3280,7 +3445,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -3288,7 +3453,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -3296,7 +3461,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -3304,7 +3469,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -3312,7 +3477,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -3320,7 +3485,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -3328,7 +3493,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -3336,7 +3501,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -3344,7 +3509,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -3352,7 +3517,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -3360,7 +3525,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -3368,7 +3533,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -3376,7 +3541,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -3384,7 +3549,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -3392,7 +3557,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -3400,7 +3565,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -3408,7 +3573,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -3416,7 +3581,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -3424,7 +3589,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -3432,7 +3597,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -3440,7 +3605,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -3448,7 +3613,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -3456,7 +3621,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -3464,7 +3629,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -3472,7 +3637,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -3480,7 +3645,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -3488,7 +3653,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -3496,7 +3661,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -3504,7 +3669,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -3512,7 +3677,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -3520,7 +3685,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -3528,7 +3693,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -3536,7 +3701,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -3544,7 +3709,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -3552,7 +3717,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -3560,7 +3725,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -3568,7 +3733,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -3576,7 +3741,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -3584,7 +3749,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
@@ -3592,7 +3757,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
@@ -3600,7 +3765,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
@@ -3608,7 +3773,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
@@ -3616,7 +3781,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>217</v>
       </c>
@@ -3624,7 +3789,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>218</v>
       </c>
@@ -3632,7 +3797,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>219</v>
       </c>
@@ -3640,7 +3805,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
@@ -3648,7 +3813,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
@@ -3656,7 +3821,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
@@ -3664,7 +3829,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
@@ -3672,7 +3837,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
@@ -3680,7 +3845,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
@@ -3688,7 +3853,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
@@ -3696,7 +3861,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
@@ -3704,7 +3869,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
@@ -3712,7 +3877,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
@@ -3720,7 +3885,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>230</v>
       </c>
@@ -3728,7 +3893,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
@@ -3736,7 +3901,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>232</v>
       </c>
@@ -3744,7 +3909,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>233</v>
       </c>
@@ -3752,7 +3917,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>234</v>
       </c>
@@ -3760,7 +3925,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>235</v>
       </c>
@@ -3768,7 +3933,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>236</v>
       </c>
@@ -3776,7 +3941,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>237</v>
       </c>
@@ -3784,7 +3949,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>238</v>
       </c>
@@ -3792,7 +3957,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>239</v>
       </c>
@@ -3800,7 +3965,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>240</v>
       </c>
@@ -3808,7 +3973,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>241</v>
       </c>
@@ -3816,7 +3981,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>242</v>
       </c>
@@ -3824,7 +3989,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>243</v>
       </c>
@@ -3832,7 +3997,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>244</v>
       </c>
@@ -3840,7 +4005,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>245</v>
       </c>
@@ -3848,7 +4013,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>246</v>
       </c>
@@ -3856,7 +4021,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>247</v>
       </c>
@@ -3864,7 +4029,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>248</v>
       </c>
@@ -3872,7 +4037,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>249</v>
       </c>
@@ -3880,7 +4045,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>
@@ -3888,7 +4053,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>251</v>
       </c>
@@ -3896,7 +4061,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>252</v>
       </c>
@@ -3904,7 +4069,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>253</v>
       </c>
@@ -3912,7 +4077,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>254</v>
       </c>
@@ -3920,7 +4085,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>255</v>
       </c>
@@ -3928,7 +4093,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>256</v>
       </c>
@@ -3936,7 +4101,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>257</v>
       </c>
@@ -3944,7 +4109,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>258</v>
       </c>
@@ -3952,7 +4117,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>259</v>
       </c>
@@ -3960,7 +4125,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>260</v>
       </c>
@@ -3968,7 +4133,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>261</v>
       </c>
@@ -3976,7 +4141,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>262</v>
       </c>
@@ -3984,7 +4149,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>263</v>
       </c>
@@ -3992,7 +4157,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>264</v>
       </c>
@@ -4000,7 +4165,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>265</v>
       </c>
@@ -4008,7 +4173,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>266</v>
       </c>
@@ -4016,7 +4181,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>267</v>
       </c>
@@ -4024,7 +4189,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>268</v>
       </c>
@@ -4032,7 +4197,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>269</v>
       </c>
@@ -4040,7 +4205,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>270</v>
       </c>
@@ -4048,7 +4213,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>271</v>
       </c>
@@ -4056,7 +4221,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>272</v>
       </c>
@@ -4064,7 +4229,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>273</v>
       </c>
@@ -4072,7 +4237,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>274</v>
       </c>
@@ -4080,7 +4245,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>275</v>
       </c>
@@ -4088,7 +4253,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>276</v>
       </c>
@@ -4096,7 +4261,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>277</v>
       </c>
@@ -4104,7 +4269,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>278</v>
       </c>
@@ -4112,7 +4277,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>279</v>
       </c>
@@ -4120,7 +4285,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>280</v>
       </c>
@@ -4128,7 +4293,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>281</v>
       </c>
@@ -4136,7 +4301,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>282</v>
       </c>
@@ -4144,7 +4309,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>283</v>
       </c>
@@ -4152,7 +4317,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>284</v>
       </c>
@@ -4160,7 +4325,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>285</v>
       </c>
@@ -4168,7 +4333,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>286</v>
       </c>
@@ -4176,7 +4341,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>287</v>
       </c>
@@ -4184,7 +4349,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>288</v>
       </c>
@@ -4192,7 +4357,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>289</v>
       </c>
@@ -4200,7 +4365,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>290</v>
       </c>
@@ -4208,7 +4373,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>291</v>
       </c>
@@ -4216,7 +4381,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>292</v>
       </c>
@@ -4224,7 +4389,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>293</v>
       </c>
@@ -4232,7 +4397,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>294</v>
       </c>
@@ -4240,7 +4405,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>295</v>
       </c>
@@ -4248,7 +4413,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>296</v>
       </c>
@@ -4256,7 +4421,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>297</v>
       </c>
@@ -4264,7 +4429,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>298</v>
       </c>
@@ -4272,7 +4437,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>299</v>
       </c>
@@ -4280,7 +4445,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>300</v>
       </c>
@@ -4288,7 +4453,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>301</v>
       </c>
@@ -4296,7 +4461,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>302</v>
       </c>
@@ -4304,7 +4469,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>303</v>
       </c>
@@ -4312,7 +4477,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>304</v>
       </c>
@@ -4320,7 +4485,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>305</v>
       </c>
@@ -4328,7 +4493,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>306</v>
       </c>
@@ -4336,7 +4501,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>307</v>
       </c>
@@ -4344,7 +4509,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>308</v>
       </c>
@@ -4352,7 +4517,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>309</v>
       </c>
@@ -4360,7 +4525,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>310</v>
       </c>
@@ -4368,7 +4533,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>311</v>
       </c>
@@ -4376,7 +4541,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>312</v>
       </c>
@@ -4384,7 +4549,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>313</v>
       </c>
@@ -4392,7 +4557,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>314</v>
       </c>
@@ -4400,7 +4565,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>315</v>
       </c>
@@ -4408,7 +4573,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>316</v>
       </c>
@@ -4416,7 +4581,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>317</v>
       </c>
@@ -4424,7 +4589,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>318</v>
       </c>
@@ -4432,7 +4597,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>319</v>
       </c>
@@ -4440,7 +4605,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>320</v>
       </c>
@@ -4448,7 +4613,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>321</v>
       </c>
@@ -4456,7 +4621,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>322</v>
       </c>
@@ -4464,7 +4629,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>323</v>
       </c>
@@ -4472,7 +4637,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>324</v>
       </c>
@@ -4480,7 +4645,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>325</v>
       </c>
@@ -4488,7 +4653,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>326</v>
       </c>
@@ -4496,7 +4661,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>327</v>
       </c>
@@ -4504,7 +4669,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>328</v>
       </c>
@@ -4512,7 +4677,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>329</v>
       </c>
@@ -4520,7 +4685,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>330</v>
       </c>
@@ -4528,7 +4693,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>331</v>
       </c>
@@ -4536,7 +4701,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>332</v>
       </c>
@@ -4544,7 +4709,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>333</v>
       </c>
@@ -4552,7 +4717,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>334</v>
       </c>
@@ -4560,7 +4725,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>335</v>
       </c>
@@ -4568,7 +4733,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>336</v>
       </c>
@@ -4586,16 +4751,16 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="30.44140625" customWidth="1"/>
-    <col min="3" max="3" width="247.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" customWidth="1"/>
+    <col min="3" max="3" width="247.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>348</v>
       </c>
@@ -4621,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4644,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4667,7 +4832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4690,7 +4855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4713,7 +4878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4736,7 +4901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4759,7 +4924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4782,7 +4947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4805,7 +4970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4828,7 +4993,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4851,7 +5016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4874,7 +5039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4897,7 +5062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4920,7 +5085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4943,7 +5108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4966,7 +5131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5003,9 +5168,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>348</v>
       </c>
@@ -5013,7 +5178,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5021,7 +5186,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5029,7 +5194,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5037,7 +5202,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -5045,7 +5210,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -5053,7 +5218,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -5061,7 +5226,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -5069,7 +5234,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -5077,7 +5242,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -5085,7 +5250,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -5093,7 +5258,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -5101,7 +5266,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -5109,7 +5274,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
@@ -5117,7 +5282,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
@@ -5125,7 +5290,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
@@ -5133,7 +5298,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
@@ -5141,7 +5306,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
@@ -5149,7 +5314,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
@@ -5157,7 +5322,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
@@ -5165,7 +5330,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
@@ -5173,7 +5338,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -5194,14 +5359,14 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>382</v>
       </c>
@@ -5209,7 +5374,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
@@ -5217,7 +5382,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>14</v>
       </c>
@@ -5225,7 +5390,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>15</v>
       </c>
@@ -5233,7 +5398,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>16</v>
       </c>
@@ -5241,7 +5406,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14</v>
       </c>
@@ -5249,7 +5414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>14</v>
       </c>
@@ -5257,7 +5422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>11</v>
       </c>
@@ -5265,7 +5430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11</v>
       </c>
@@ -5273,7 +5438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -5281,7 +5446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
@@ -5289,7 +5454,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -5297,7 +5462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -5314,16 +5479,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>348</v>
       </c>
@@ -5332,7 +5497,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -5340,7 +5505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -5348,7 +5513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -5356,7 +5521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -5364,7 +5529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -5372,7 +5537,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -5380,7 +5545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>2</v>
       </c>
@@ -5388,7 +5553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -5396,7 +5561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>2</v>
       </c>
@@ -5404,7 +5569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>2</v>
       </c>
@@ -5412,7 +5577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>2</v>
       </c>
@@ -5420,7 +5585,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -5428,7 +5593,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -5436,7 +5601,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
@@ -5444,7 +5609,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -5452,7 +5617,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -5460,7 +5625,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
@@ -5468,7 +5633,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
@@ -5476,7 +5641,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -5484,7 +5649,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
@@ -5492,7 +5657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9</v>
       </c>
@@ -5500,7 +5665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>9</v>
       </c>
@@ -5508,7 +5673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
@@ -5516,7 +5681,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
@@ -5524,7 +5689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>10</v>
       </c>
@@ -5532,7 +5697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>10</v>
       </c>
@@ -5540,7 +5705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10</v>
       </c>
@@ -5548,7 +5713,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11</v>
       </c>
@@ -5556,7 +5721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>11</v>
       </c>
@@ -5564,7 +5729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>11</v>
       </c>
@@ -5572,7 +5737,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>11</v>
       </c>
@@ -5580,7 +5745,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>12</v>
       </c>
@@ -5588,7 +5753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>12</v>
       </c>
@@ -5596,7 +5761,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>12</v>
       </c>
@@ -5604,7 +5769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>12</v>
       </c>
@@ -5612,7 +5777,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>13</v>
       </c>
@@ -5620,7 +5785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>13</v>
       </c>
@@ -5628,7 +5793,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>13</v>
       </c>
@@ -5636,7 +5801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>13</v>
       </c>
@@ -5644,7 +5809,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>14</v>
       </c>
@@ -5652,7 +5817,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>14</v>
       </c>
@@ -5660,7 +5825,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>15</v>
       </c>
@@ -5668,7 +5833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>15</v>
       </c>
@@ -5677,7 +5842,7 @@
       </c>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>16</v>
       </c>
@@ -5686,7 +5851,7 @@
       </c>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>16</v>
       </c>
@@ -5703,21 +5868,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="78.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="78.28515625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>388</v>
       </c>
@@ -5743,7 +5910,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>395</v>
       </c>
@@ -5766,7 +5933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>398</v>
       </c>
@@ -5789,7 +5956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>401</v>
       </c>
@@ -5812,7 +5979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>403</v>
       </c>
@@ -5835,7 +6002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>409</v>
       </c>
@@ -5858,7 +6025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>412</v>
       </c>
@@ -5881,7 +6048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>413</v>
       </c>
@@ -5901,10 +6068,10 @@
         <v>20121112</v>
       </c>
       <c r="H8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>414</v>
       </c>
@@ -5924,10 +6091,10 @@
         <v>20121112</v>
       </c>
       <c r="H9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>421</v>
       </c>
@@ -5947,10 +6114,10 @@
         <v>20121112</v>
       </c>
       <c r="H10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>422</v>
       </c>
@@ -5973,7 +6140,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>423</v>
       </c>
@@ -5993,10 +6160,10 @@
         <v>20121112</v>
       </c>
       <c r="H12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>424</v>
       </c>
@@ -6016,10 +6183,10 @@
         <v>20121112</v>
       </c>
       <c r="H13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>426</v>
       </c>
@@ -6039,10 +6206,10 @@
         <v>20121112</v>
       </c>
       <c r="H14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>425</v>
       </c>
@@ -6065,6 +6232,492 @@
         <v>5</v>
       </c>
       <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>439</v>
+      </c>
+      <c r="B16" t="s">
+        <v>440</v>
+      </c>
+      <c r="C16" t="s">
+        <v>441</v>
+      </c>
+      <c r="D16" t="s">
+        <v>400</v>
+      </c>
+      <c r="E16">
+        <v>20130105</v>
+      </c>
+      <c r="F16">
+        <v>20140530</v>
+      </c>
+      <c r="H16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>442</v>
+      </c>
+      <c r="B17" t="s">
+        <v>443</v>
+      </c>
+      <c r="C17" t="s">
+        <v>452</v>
+      </c>
+      <c r="D17" t="s">
+        <v>400</v>
+      </c>
+      <c r="E17">
+        <v>20140110</v>
+      </c>
+      <c r="F17">
+        <v>20140530</v>
+      </c>
+      <c r="H17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>444</v>
+      </c>
+      <c r="B18" t="s">
+        <v>446</v>
+      </c>
+      <c r="C18" t="s">
+        <v>448</v>
+      </c>
+      <c r="D18" t="s">
+        <v>400</v>
+      </c>
+      <c r="E18">
+        <v>20130105</v>
+      </c>
+      <c r="F18">
+        <v>20140530</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>445</v>
+      </c>
+      <c r="B19" t="s">
+        <v>447</v>
+      </c>
+      <c r="C19" t="s">
+        <v>453</v>
+      </c>
+      <c r="D19" t="s">
+        <v>400</v>
+      </c>
+      <c r="E19">
+        <v>20140110</v>
+      </c>
+      <c r="F19">
+        <v>20140530</v>
+      </c>
+      <c r="H19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>449</v>
+      </c>
+      <c r="B20" t="s">
+        <v>456</v>
+      </c>
+      <c r="C20" t="s">
+        <v>451</v>
+      </c>
+      <c r="D20" t="s">
+        <v>400</v>
+      </c>
+      <c r="E20">
+        <v>20130105</v>
+      </c>
+      <c r="F20">
+        <v>20140530</v>
+      </c>
+      <c r="H20">
+        <v>8</v>
+      </c>
+      <c r="J20" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>450</v>
+      </c>
+      <c r="B21" t="s">
+        <v>455</v>
+      </c>
+      <c r="C21" t="s">
+        <v>454</v>
+      </c>
+      <c r="D21" t="s">
+        <v>400</v>
+      </c>
+      <c r="E21">
+        <v>20140110</v>
+      </c>
+      <c r="F21">
+        <v>20140530</v>
+      </c>
+      <c r="H21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>458</v>
+      </c>
+      <c r="B22" t="s">
+        <v>459</v>
+      </c>
+      <c r="C22" t="s">
+        <v>460</v>
+      </c>
+      <c r="D22" t="s">
+        <v>397</v>
+      </c>
+      <c r="E22">
+        <v>20001103</v>
+      </c>
+      <c r="F22">
+        <v>20050211</v>
+      </c>
+      <c r="H22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>461</v>
+      </c>
+      <c r="B23" t="s">
+        <v>462</v>
+      </c>
+      <c r="C23" t="s">
+        <v>463</v>
+      </c>
+      <c r="D23" t="s">
+        <v>400</v>
+      </c>
+      <c r="E23">
+        <v>20030115</v>
+      </c>
+      <c r="F23">
+        <v>20050211</v>
+      </c>
+      <c r="H23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>464</v>
+      </c>
+      <c r="B24" t="s">
+        <v>465</v>
+      </c>
+      <c r="C24" t="s">
+        <v>466</v>
+      </c>
+      <c r="D24" t="s">
+        <v>400</v>
+      </c>
+      <c r="E24">
+        <v>20081201</v>
+      </c>
+      <c r="F24">
+        <v>20101207</v>
+      </c>
+      <c r="H24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>467</v>
+      </c>
+      <c r="B25" t="s">
+        <v>468</v>
+      </c>
+      <c r="C25" t="s">
+        <v>469</v>
+      </c>
+      <c r="D25" t="s">
+        <v>400</v>
+      </c>
+      <c r="E25">
+        <v>20130905</v>
+      </c>
+      <c r="F25">
+        <v>20140912</v>
+      </c>
+      <c r="H25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>470</v>
+      </c>
+      <c r="B26" t="s">
+        <v>471</v>
+      </c>
+      <c r="C26" t="s">
+        <v>472</v>
+      </c>
+      <c r="D26" t="s">
+        <v>400</v>
+      </c>
+      <c r="E26">
+        <v>20131206</v>
+      </c>
+      <c r="F26">
+        <v>20140912</v>
+      </c>
+      <c r="H26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>473</v>
+      </c>
+      <c r="B27" t="s">
+        <v>477</v>
+      </c>
+      <c r="C27" t="s">
+        <v>469</v>
+      </c>
+      <c r="D27" t="s">
+        <v>400</v>
+      </c>
+      <c r="E27">
+        <v>20130905</v>
+      </c>
+      <c r="F27">
+        <v>20140912</v>
+      </c>
+      <c r="H27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>474</v>
+      </c>
+      <c r="B28" t="s">
+        <v>478</v>
+      </c>
+      <c r="C28" t="s">
+        <v>472</v>
+      </c>
+      <c r="D28" t="s">
+        <v>400</v>
+      </c>
+      <c r="E28">
+        <v>20131206</v>
+      </c>
+      <c r="F28">
+        <v>20140912</v>
+      </c>
+      <c r="H28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>476</v>
+      </c>
+      <c r="B29" t="s">
+        <v>479</v>
+      </c>
+      <c r="C29" t="s">
+        <v>469</v>
+      </c>
+      <c r="D29" t="s">
+        <v>400</v>
+      </c>
+      <c r="E29">
+        <v>20130905</v>
+      </c>
+      <c r="F29">
+        <v>20140912</v>
+      </c>
+      <c r="H29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>475</v>
+      </c>
+      <c r="B30" t="s">
+        <v>480</v>
+      </c>
+      <c r="C30" t="s">
+        <v>472</v>
+      </c>
+      <c r="D30" t="s">
+        <v>400</v>
+      </c>
+      <c r="E30">
+        <v>20131206</v>
+      </c>
+      <c r="F30">
+        <v>20140912</v>
+      </c>
+      <c r="H30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>481</v>
+      </c>
+      <c r="B31" t="s">
+        <v>487</v>
+      </c>
+      <c r="C31" t="s">
+        <v>493</v>
+      </c>
+      <c r="D31" t="s">
+        <v>400</v>
+      </c>
+      <c r="E31">
+        <v>20120905</v>
+      </c>
+      <c r="F31">
+        <v>20130913</v>
+      </c>
+      <c r="H31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>482</v>
+      </c>
+      <c r="B32" t="s">
+        <v>488</v>
+      </c>
+      <c r="C32" t="s">
+        <v>472</v>
+      </c>
+      <c r="D32" t="s">
+        <v>400</v>
+      </c>
+      <c r="E32">
+        <v>20121206</v>
+      </c>
+      <c r="F32">
+        <v>20130913</v>
+      </c>
+      <c r="H32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>483</v>
+      </c>
+      <c r="B33" t="s">
+        <v>489</v>
+      </c>
+      <c r="C33" t="s">
+        <v>493</v>
+      </c>
+      <c r="D33" t="s">
+        <v>400</v>
+      </c>
+      <c r="E33">
+        <v>20120905</v>
+      </c>
+      <c r="F33">
+        <v>20130913</v>
+      </c>
+      <c r="H33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>484</v>
+      </c>
+      <c r="B34" t="s">
+        <v>490</v>
+      </c>
+      <c r="C34" t="s">
+        <v>472</v>
+      </c>
+      <c r="D34" t="s">
+        <v>400</v>
+      </c>
+      <c r="E34">
+        <v>20121206</v>
+      </c>
+      <c r="F34">
+        <v>20130913</v>
+      </c>
+      <c r="H34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>485</v>
+      </c>
+      <c r="B35" t="s">
+        <v>491</v>
+      </c>
+      <c r="C35" t="s">
+        <v>493</v>
+      </c>
+      <c r="D35" t="s">
+        <v>400</v>
+      </c>
+      <c r="E35">
+        <v>20120905</v>
+      </c>
+      <c r="F35">
+        <v>20130913</v>
+      </c>
+      <c r="H35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>486</v>
+      </c>
+      <c r="B36" t="s">
+        <v>492</v>
+      </c>
+      <c r="C36" t="s">
+        <v>472</v>
+      </c>
+      <c r="D36" t="s">
+        <v>400</v>
+      </c>
+      <c r="E36">
+        <v>20121206</v>
+      </c>
+      <c r="F36">
+        <v>20130913</v>
+      </c>
+      <c r="H36">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
JE commentaire tblTheme et tblGenre
j'en ai fait quelque un
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Utilisateur\Dropbox\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Dropbox\Projet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" tabRatio="633" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="633" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="tblMode" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="500">
   <si>
     <t>IdMode</t>
   </si>
@@ -1512,6 +1512,24 @@
   </si>
   <si>
     <t>1er version, nouveau joueur, peu de bug, ressemblance avec NHL 2013</t>
+  </si>
+  <si>
+    <t>Un jeu où pratiquement  tout tourne autour des voiture</t>
+  </si>
+  <si>
+    <t>Une adaptation d'un roman sous format vidéoludique</t>
+  </si>
+  <si>
+    <t>Un jeu qui tourne autour des combats, gladiateur, guerre, etc</t>
+  </si>
+  <si>
+    <t>Je ne comprend pas ces quoi la diffèrence avec l'autre</t>
+  </si>
+  <si>
+    <t>Pour les jeu qui ne comporte que du billard, pas comme un mini-jeux</t>
+  </si>
+  <si>
+    <t>Les jeux avec des beaux chapeaux</t>
   </si>
 </sst>
 </file>
@@ -1962,13 +1980,13 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="106.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="106.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1979,7 +1997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16.899999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1990,7 +2008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2001,7 +2019,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2012,7 +2030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2033,16 +2051,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C337"/>
   <sheetViews>
-    <sheetView topLeftCell="A334" workbookViewId="0">
-      <selection activeCell="C165" sqref="C165"/>
+    <sheetView topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="C335" sqref="C335"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" customWidth="1"/>
+    <col min="3" max="3" width="57.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2053,7 +2072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2061,7 +2080,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2069,23 +2088,29 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2093,7 +2118,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2101,7 +2126,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2109,7 +2134,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2117,7 +2142,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2125,7 +2150,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2133,7 +2158,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2141,7 +2166,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2149,7 +2174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2157,7 +2182,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2165,7 +2190,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2173,7 +2198,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2181,7 +2206,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2189,7 +2214,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2197,7 +2222,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2205,7 +2230,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2213,7 +2238,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2221,7 +2246,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2229,7 +2254,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2237,7 +2262,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2245,7 +2270,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2253,7 +2278,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2261,15 +2286,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2277,7 +2305,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2285,15 +2313,18 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2301,7 +2332,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2309,7 +2340,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2317,7 +2348,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2325,7 +2356,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2333,7 +2364,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2341,7 +2372,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2349,15 +2380,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2365,7 +2399,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2373,7 +2407,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2381,7 +2415,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2389,7 +2423,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2397,7 +2431,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2405,7 +2439,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2413,7 +2447,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2421,7 +2455,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2429,7 +2463,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2437,7 +2471,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2445,7 +2479,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2453,7 +2487,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2461,7 +2495,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2469,7 +2503,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2477,7 +2511,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2485,7 +2519,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2493,7 +2527,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2501,7 +2535,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2509,7 +2543,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2517,7 +2551,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2525,7 +2559,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2533,7 +2567,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2541,7 +2575,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2549,7 +2583,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2557,7 +2591,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2565,7 +2599,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2573,7 +2607,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2581,7 +2615,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2589,7 +2623,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2597,7 +2631,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2605,7 +2639,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2613,7 +2647,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2621,7 +2655,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2629,7 +2663,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2637,7 +2671,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2645,7 +2679,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2653,7 +2687,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2661,7 +2695,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2669,7 +2703,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2677,7 +2711,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2685,7 +2719,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -2693,7 +2727,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -2701,7 +2735,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -2709,7 +2743,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -2717,7 +2751,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -2725,7 +2759,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -2733,7 +2767,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -2741,7 +2775,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -2749,7 +2783,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2757,7 +2791,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2765,7 +2799,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2773,7 +2807,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2781,7 +2815,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2789,7 +2823,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2797,7 +2831,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2805,7 +2839,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2813,7 +2847,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2821,7 +2855,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -2829,7 +2863,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -2837,7 +2871,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -2845,7 +2879,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -2853,7 +2887,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -2861,7 +2895,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -2869,7 +2903,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -2877,7 +2911,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -2885,7 +2919,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -2893,7 +2927,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -2901,7 +2935,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -2909,7 +2943,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -2917,7 +2951,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -2925,7 +2959,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2933,7 +2967,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2941,7 +2975,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2949,7 +2983,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2957,7 +2991,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2965,7 +2999,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2973,7 +3007,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2981,7 +3015,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2989,7 +3023,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2997,7 +3031,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -3005,7 +3039,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -3013,7 +3047,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -3021,7 +3055,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -3029,7 +3063,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -3037,7 +3071,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -3045,7 +3079,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -3053,7 +3087,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -3061,7 +3095,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -3069,7 +3103,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -3077,7 +3111,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -3085,7 +3119,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -3093,7 +3127,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -3101,7 +3135,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -3109,7 +3143,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -3117,7 +3151,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -3125,7 +3159,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -3133,7 +3167,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -3141,7 +3175,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -3149,7 +3183,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -3157,7 +3191,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -3165,7 +3199,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -3173,7 +3207,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -3181,7 +3215,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -3189,7 +3223,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -3197,7 +3231,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -3205,7 +3239,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -3213,7 +3247,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
@@ -3221,7 +3255,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
@@ -3229,7 +3263,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
@@ -3237,7 +3271,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
@@ -3245,7 +3279,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
@@ -3253,7 +3287,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
@@ -3261,7 +3295,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
@@ -3269,7 +3303,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
@@ -3277,7 +3311,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
@@ -3285,7 +3319,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
@@ -3293,7 +3327,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
@@ -3301,7 +3335,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
@@ -3309,7 +3343,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>158</v>
       </c>
@@ -3317,7 +3351,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>159</v>
       </c>
@@ -3325,7 +3359,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
@@ -3333,7 +3367,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
@@ -3341,7 +3375,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
@@ -3349,7 +3383,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
@@ -3357,7 +3391,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
@@ -3365,7 +3399,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
@@ -3373,7 +3407,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -3381,7 +3415,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -3389,7 +3423,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -3397,7 +3431,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -3405,7 +3439,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -3413,7 +3447,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -3421,7 +3455,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -3429,7 +3463,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
@@ -3437,7 +3471,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
@@ -3445,7 +3479,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
@@ -3453,7 +3487,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
@@ -3461,7 +3495,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
@@ -3469,7 +3503,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
@@ -3477,7 +3511,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
@@ -3485,7 +3519,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
@@ -3493,7 +3527,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
@@ -3501,7 +3535,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
@@ -3509,7 +3543,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
@@ -3517,7 +3551,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
@@ -3525,7 +3559,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
@@ -3533,7 +3567,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
@@ -3541,7 +3575,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
@@ -3549,7 +3583,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>188</v>
       </c>
@@ -3557,7 +3591,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>189</v>
       </c>
@@ -3565,7 +3599,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>190</v>
       </c>
@@ -3573,7 +3607,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>191</v>
       </c>
@@ -3581,7 +3615,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>192</v>
       </c>
@@ -3589,7 +3623,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>193</v>
       </c>
@@ -3597,7 +3631,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>194</v>
       </c>
@@ -3605,7 +3639,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>195</v>
       </c>
@@ -3613,7 +3647,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>196</v>
       </c>
@@ -3621,7 +3655,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>197</v>
       </c>
@@ -3629,7 +3663,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>198</v>
       </c>
@@ -3637,7 +3671,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>199</v>
       </c>
@@ -3645,7 +3679,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>200</v>
       </c>
@@ -3653,7 +3687,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>201</v>
       </c>
@@ -3661,7 +3695,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>202</v>
       </c>
@@ -3669,7 +3703,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>203</v>
       </c>
@@ -3677,7 +3711,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>204</v>
       </c>
@@ -3685,7 +3719,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>205</v>
       </c>
@@ -3693,7 +3727,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>206</v>
       </c>
@@ -3701,7 +3735,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>207</v>
       </c>
@@ -3709,7 +3743,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
@@ -3717,7 +3751,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
@@ -3725,7 +3759,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
@@ -3733,7 +3767,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
@@ -3741,7 +3775,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
@@ -3749,7 +3783,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
@@ -3757,7 +3791,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
@@ -3765,7 +3799,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
@@ -3773,7 +3807,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
@@ -3781,7 +3815,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
@@ -3789,7 +3823,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
@@ -3797,7 +3831,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
@@ -3805,7 +3839,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
@@ -3813,7 +3847,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
@@ -3821,7 +3855,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
@@ -3829,7 +3863,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
@@ -3837,7 +3871,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>224</v>
       </c>
@@ -3845,7 +3879,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>225</v>
       </c>
@@ -3853,7 +3887,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>226</v>
       </c>
@@ -3861,7 +3895,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>227</v>
       </c>
@@ -3869,7 +3903,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>228</v>
       </c>
@@ -3877,7 +3911,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>229</v>
       </c>
@@ -3885,7 +3919,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>230</v>
       </c>
@@ -3893,7 +3927,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>231</v>
       </c>
@@ -3901,7 +3935,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>232</v>
       </c>
@@ -3909,7 +3943,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>233</v>
       </c>
@@ -3917,7 +3951,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>234</v>
       </c>
@@ -3925,7 +3959,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>235</v>
       </c>
@@ -3933,7 +3967,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>236</v>
       </c>
@@ -3941,7 +3975,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>237</v>
       </c>
@@ -3949,7 +3983,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>238</v>
       </c>
@@ -3957,7 +3991,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>239</v>
       </c>
@@ -3965,7 +3999,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>240</v>
       </c>
@@ -3973,7 +4007,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>241</v>
       </c>
@@ -3981,7 +4015,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>242</v>
       </c>
@@ -3989,7 +4023,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>243</v>
       </c>
@@ -3997,7 +4031,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>244</v>
       </c>
@@ -4005,7 +4039,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>245</v>
       </c>
@@ -4013,7 +4047,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>246</v>
       </c>
@@ -4021,7 +4055,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>247</v>
       </c>
@@ -4029,7 +4063,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>248</v>
       </c>
@@ -4037,7 +4071,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>249</v>
       </c>
@@ -4045,7 +4079,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>250</v>
       </c>
@@ -4053,7 +4087,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>251</v>
       </c>
@@ -4061,7 +4095,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>252</v>
       </c>
@@ -4069,7 +4103,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>253</v>
       </c>
@@ -4077,7 +4111,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>254</v>
       </c>
@@ -4085,7 +4119,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>255</v>
       </c>
@@ -4093,7 +4127,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>256</v>
       </c>
@@ -4101,7 +4135,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>257</v>
       </c>
@@ -4109,7 +4143,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>258</v>
       </c>
@@ -4117,7 +4151,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>259</v>
       </c>
@@ -4125,7 +4159,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>260</v>
       </c>
@@ -4133,7 +4167,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>261</v>
       </c>
@@ -4141,7 +4175,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>262</v>
       </c>
@@ -4149,7 +4183,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>263</v>
       </c>
@@ -4157,7 +4191,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>264</v>
       </c>
@@ -4165,7 +4199,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>265</v>
       </c>
@@ -4173,7 +4207,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>266</v>
       </c>
@@ -4181,7 +4215,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>267</v>
       </c>
@@ -4189,7 +4223,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>268</v>
       </c>
@@ -4197,7 +4231,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>269</v>
       </c>
@@ -4205,7 +4239,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>270</v>
       </c>
@@ -4213,7 +4247,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>271</v>
       </c>
@@ -4221,7 +4255,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>272</v>
       </c>
@@ -4229,7 +4263,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>273</v>
       </c>
@@ -4237,7 +4271,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>274</v>
       </c>
@@ -4245,7 +4279,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>275</v>
       </c>
@@ -4253,7 +4287,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>276</v>
       </c>
@@ -4261,7 +4295,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>277</v>
       </c>
@@ -4269,7 +4303,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>278</v>
       </c>
@@ -4277,7 +4311,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>279</v>
       </c>
@@ -4285,7 +4319,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>280</v>
       </c>
@@ -4293,7 +4327,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>281</v>
       </c>
@@ -4301,7 +4335,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>282</v>
       </c>
@@ -4309,7 +4343,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>283</v>
       </c>
@@ -4317,7 +4351,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>284</v>
       </c>
@@ -4325,7 +4359,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>285</v>
       </c>
@@ -4333,7 +4367,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>286</v>
       </c>
@@ -4341,7 +4375,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>287</v>
       </c>
@@ -4349,7 +4383,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>288</v>
       </c>
@@ -4357,7 +4391,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>289</v>
       </c>
@@ -4365,7 +4399,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>290</v>
       </c>
@@ -4373,7 +4407,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>291</v>
       </c>
@@ -4381,7 +4415,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>292</v>
       </c>
@@ -4389,7 +4423,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>293</v>
       </c>
@@ -4397,7 +4431,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>294</v>
       </c>
@@ -4405,7 +4439,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>295</v>
       </c>
@@ -4413,7 +4447,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>296</v>
       </c>
@@ -4421,7 +4455,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>297</v>
       </c>
@@ -4429,7 +4463,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>298</v>
       </c>
@@ -4437,7 +4471,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>299</v>
       </c>
@@ -4445,7 +4479,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>300</v>
       </c>
@@ -4453,7 +4487,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>301</v>
       </c>
@@ -4461,7 +4495,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>302</v>
       </c>
@@ -4469,7 +4503,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>303</v>
       </c>
@@ -4477,7 +4511,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>304</v>
       </c>
@@ -4485,7 +4519,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>305</v>
       </c>
@@ -4493,7 +4527,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>306</v>
       </c>
@@ -4501,7 +4535,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>307</v>
       </c>
@@ -4509,7 +4543,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>308</v>
       </c>
@@ -4517,7 +4551,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>309</v>
       </c>
@@ -4525,7 +4559,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>310</v>
       </c>
@@ -4533,7 +4567,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>311</v>
       </c>
@@ -4541,7 +4575,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>312</v>
       </c>
@@ -4549,7 +4583,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>313</v>
       </c>
@@ -4557,7 +4591,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>314</v>
       </c>
@@ -4565,7 +4599,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>315</v>
       </c>
@@ -4573,7 +4607,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>316</v>
       </c>
@@ -4581,7 +4615,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>317</v>
       </c>
@@ -4589,7 +4623,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>318</v>
       </c>
@@ -4597,7 +4631,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>319</v>
       </c>
@@ -4605,7 +4639,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>320</v>
       </c>
@@ -4613,7 +4647,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>321</v>
       </c>
@@ -4621,7 +4655,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>322</v>
       </c>
@@ -4629,7 +4663,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>323</v>
       </c>
@@ -4637,7 +4671,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>324</v>
       </c>
@@ -4645,7 +4679,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>325</v>
       </c>
@@ -4653,7 +4687,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>326</v>
       </c>
@@ -4661,7 +4695,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>327</v>
       </c>
@@ -4669,7 +4703,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>328</v>
       </c>
@@ -4677,7 +4711,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>329</v>
       </c>
@@ -4685,7 +4719,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>330</v>
       </c>
@@ -4693,7 +4727,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>331</v>
       </c>
@@ -4701,7 +4735,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>332</v>
       </c>
@@ -4709,7 +4743,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>333</v>
       </c>
@@ -4717,15 +4751,18 @@
         <v>344</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>334</v>
       </c>
       <c r="B335" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C335" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>335</v>
       </c>
@@ -4733,7 +4770,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>336</v>
       </c>
@@ -4750,17 +4787,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="247.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.44140625" customWidth="1"/>
+    <col min="3" max="3" width="247.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>348</v>
       </c>
@@ -4786,7 +4823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4809,7 +4846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4832,7 +4869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4855,7 +4892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4878,7 +4915,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4901,7 +4938,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4924,7 +4961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4947,7 +4984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4970,7 +5007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4993,7 +5030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5016,7 +5053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5039,7 +5076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5062,7 +5099,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5085,7 +5122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5108,7 +5145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5131,7 +5168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5168,9 +5205,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>348</v>
       </c>
@@ -5178,7 +5215,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5186,7 +5223,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5194,7 +5231,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5202,7 +5239,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -5210,7 +5247,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -5218,7 +5255,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -5226,7 +5263,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -5234,7 +5271,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -5242,7 +5279,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -5250,7 +5287,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>5</v>
       </c>
@@ -5258,7 +5295,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -5266,7 +5303,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>7</v>
       </c>
@@ -5274,7 +5311,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
@@ -5282,7 +5319,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9</v>
       </c>
@@ -5290,7 +5327,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
@@ -5298,7 +5335,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>11</v>
       </c>
@@ -5306,7 +5343,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>12</v>
       </c>
@@ -5314,7 +5351,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>13</v>
       </c>
@@ -5322,7 +5359,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>14</v>
       </c>
@@ -5330,7 +5367,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>15</v>
       </c>
@@ -5338,7 +5375,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>16</v>
       </c>
@@ -5359,14 +5396,14 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>382</v>
       </c>
@@ -5374,7 +5411,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>9</v>
       </c>
@@ -5382,7 +5419,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>14</v>
       </c>
@@ -5390,7 +5427,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>15</v>
       </c>
@@ -5398,7 +5435,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>16</v>
       </c>
@@ -5406,7 +5443,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>14</v>
       </c>
@@ -5414,7 +5451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>14</v>
       </c>
@@ -5422,7 +5459,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>11</v>
       </c>
@@ -5430,7 +5467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>11</v>
       </c>
@@ -5438,7 +5475,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -5446,7 +5483,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>3</v>
       </c>
@@ -5454,7 +5491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>6</v>
       </c>
@@ -5462,7 +5499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -5479,16 +5516,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>348</v>
       </c>
@@ -5497,7 +5534,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>1</v>
       </c>
@@ -5505,7 +5542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -5513,7 +5550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1</v>
       </c>
@@ -5521,7 +5558,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -5529,7 +5566,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -5537,7 +5574,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>2</v>
       </c>
@@ -5545,7 +5582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>2</v>
       </c>
@@ -5553,7 +5590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>2</v>
       </c>
@@ -5561,7 +5598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>2</v>
       </c>
@@ -5569,7 +5606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>2</v>
       </c>
@@ -5577,7 +5614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>2</v>
       </c>
@@ -5585,7 +5622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -5593,7 +5630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -5601,7 +5638,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>3</v>
       </c>
@@ -5609,7 +5646,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>4</v>
       </c>
@@ -5617,7 +5654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
@@ -5625,7 +5662,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>6</v>
       </c>
@@ -5633,7 +5670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>7</v>
       </c>
@@ -5641,7 +5678,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>8</v>
       </c>
@@ -5649,7 +5686,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>9</v>
       </c>
@@ -5657,7 +5694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9</v>
       </c>
@@ -5665,7 +5702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>9</v>
       </c>
@@ -5673,7 +5710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>9</v>
       </c>
@@ -5681,7 +5718,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>10</v>
       </c>
@@ -5689,7 +5726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>10</v>
       </c>
@@ -5697,7 +5734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>10</v>
       </c>
@@ -5705,7 +5742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>10</v>
       </c>
@@ -5713,7 +5750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>11</v>
       </c>
@@ -5721,7 +5758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>11</v>
       </c>
@@ -5729,7 +5766,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>11</v>
       </c>
@@ -5737,7 +5774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>11</v>
       </c>
@@ -5745,7 +5782,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>12</v>
       </c>
@@ -5753,7 +5790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>12</v>
       </c>
@@ -5761,7 +5798,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>12</v>
       </c>
@@ -5769,7 +5806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>12</v>
       </c>
@@ -5777,7 +5814,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>13</v>
       </c>
@@ -5785,7 +5822,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>13</v>
       </c>
@@ -5793,7 +5830,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>13</v>
       </c>
@@ -5801,7 +5838,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>13</v>
       </c>
@@ -5809,7 +5846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>14</v>
       </c>
@@ -5817,7 +5854,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>14</v>
       </c>
@@ -5825,7 +5862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>15</v>
       </c>
@@ -5833,7 +5870,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>15</v>
       </c>
@@ -5842,7 +5879,7 @@
       </c>
       <c r="C44" s="4"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>16</v>
       </c>
@@ -5851,7 +5888,7 @@
       </c>
       <c r="C45" s="4"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>16</v>
       </c>
@@ -5870,21 +5907,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="78.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="78.33203125" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>388</v>
       </c>
@@ -5910,7 +5947,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>395</v>
       </c>
@@ -5933,7 +5970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>398</v>
       </c>
@@ -5956,7 +5993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>401</v>
       </c>
@@ -5979,7 +6016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>403</v>
       </c>
@@ -6002,7 +6039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>409</v>
       </c>
@@ -6025,7 +6062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>412</v>
       </c>
@@ -6048,7 +6085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>413</v>
       </c>
@@ -6071,7 +6108,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>414</v>
       </c>
@@ -6094,7 +6131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>421</v>
       </c>
@@ -6117,7 +6154,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>422</v>
       </c>
@@ -6140,7 +6177,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>423</v>
       </c>
@@ -6163,7 +6200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>424</v>
       </c>
@@ -6186,7 +6223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>426</v>
       </c>
@@ -6209,7 +6246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>425</v>
       </c>
@@ -6233,7 +6270,7 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>439</v>
       </c>
@@ -6256,7 +6293,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>442</v>
       </c>
@@ -6279,7 +6316,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>444</v>
       </c>
@@ -6302,7 +6339,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>445</v>
       </c>
@@ -6325,7 +6362,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>449</v>
       </c>
@@ -6351,7 +6388,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>450</v>
       </c>
@@ -6374,7 +6411,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>458</v>
       </c>
@@ -6397,7 +6434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>461</v>
       </c>
@@ -6420,7 +6457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>464</v>
       </c>
@@ -6443,7 +6480,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>467</v>
       </c>
@@ -6466,7 +6503,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>470</v>
       </c>
@@ -6489,7 +6526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>473</v>
       </c>
@@ -6512,7 +6549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>474</v>
       </c>
@@ -6535,7 +6572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>476</v>
       </c>
@@ -6558,7 +6595,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>475</v>
       </c>
@@ -6581,7 +6618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>481</v>
       </c>
@@ -6604,7 +6641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>482</v>
       </c>
@@ -6627,7 +6664,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>483</v>
       </c>
@@ -6650,7 +6687,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>484</v>
       </c>
@@ -6673,7 +6710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>485</v>
       </c>
@@ -6696,7 +6733,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>486</v>
       </c>

</xml_diff>

<commit_message>
mise a jour JE globale
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01-JE-06_Jeu_etc.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="633" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408" tabRatio="633" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="tblMode" sheetId="1" r:id="rId1"/>
@@ -5201,7 +5201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9:E10"/>
     </sheetView>
   </sheetViews>
@@ -5516,7 +5516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>